<commit_message>
Writing dispersions in Excel
</commit_message>
<xml_diff>
--- a/lab2/краб.xlsx
+++ b/lab2/краб.xlsx
@@ -12,18 +12,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>John</t>
+    <t xml:space="preserve">Dispersion in X column: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dispersion in Y column: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dispersion in Z column: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -53,30 +57,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="2" max="2" width="11.0703125" customWidth="true" bestFit="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>40492.0</v>
+      <c r="B1" t="n">
+        <v>0.30020066935891704</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0.053782220004107456</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="n">
+        <v>7.427918040272801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
List chooser by index
</commit_message>
<xml_diff>
--- a/lab2/краб.xlsx
+++ b/lab2/краб.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Среднее геометрическое для 1-й выборки: </t>
   </si>
@@ -23,9 +23,6 @@
     <t xml:space="preserve">Среднее геометрическое для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Среднее геометрическое для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Среднее арифметическое для 1-й выборки: </t>
   </si>
   <si>
@@ -35,9 +32,6 @@
     <t xml:space="preserve">Среднее арифметическое для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Среднее арифметическое для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Оценка стандартного отклонения для 1-й выборки: </t>
   </si>
   <si>
@@ -47,9 +41,6 @@
     <t xml:space="preserve">Оценка стандартного отклонения для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Оценка стандартного отклонения для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Размах для 1-й выборки: </t>
   </si>
   <si>
@@ -59,9 +50,6 @@
     <t xml:space="preserve">Размах для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Размах для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Коэффициент ковариации с последующей выборкой для 1-й выборки: </t>
   </si>
   <si>
@@ -71,9 +59,6 @@
     <t xml:space="preserve">Коэффициент ковариации с последующей выборкой для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Коэффициент ковариации с последующей выборкой для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Количество элементов для 1-й выборки: </t>
   </si>
   <si>
@@ -83,9 +68,6 @@
     <t xml:space="preserve">Количество элементов для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Количество элементов для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Коэффициент варации для 1-й выборки: </t>
   </si>
   <si>
@@ -95,9 +77,6 @@
     <t xml:space="preserve">Коэффициент варации для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Коэффициент варации для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Нижняя граница доверительного интервала для 1-й выборки: </t>
   </si>
   <si>
@@ -107,9 +86,6 @@
     <t xml:space="preserve">Нижняя граница доверительного интервала для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Нижняя граница доверительного интервала для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Верхняя граница доверительного интервала для 1-й выборки: </t>
   </si>
   <si>
@@ -119,9 +95,6 @@
     <t xml:space="preserve">Верхняя граница доверительного интервала для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Верхняя граница доверительного интервала для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Оценка дисперсии для 1-й выборки: </t>
   </si>
   <si>
@@ -131,9 +104,6 @@
     <t xml:space="preserve">Оценка дисперсии для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Оценка дисперсии для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Максимум для 1-й выборки: </t>
   </si>
   <si>
@@ -143,9 +113,6 @@
     <t xml:space="preserve">Максимум для 3-й выборки: </t>
   </si>
   <si>
-    <t xml:space="preserve">Максимум для 4-й выборки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Минимум для 1-й выборки: </t>
   </si>
   <si>
@@ -153,9 +120,6 @@
   </si>
   <si>
     <t xml:space="preserve">Минимум для 3-й выборки: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Минимум для 4-й выборки: </t>
   </si>
 </sst>
 </file>
@@ -200,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -211,9 +175,7 @@
     <col min="3" max="3" width="49.74609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.8515625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="67.71875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="12.73828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="67.71875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.8515625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.8515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -227,7 +189,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>0.48372825699130767</v>
+        <v>0.5490716333494366</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -235,297 +197,225 @@
       <c r="F1" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="e">
-        <v>#NUM!</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.08575586070772259</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.027285504611209023</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="n">
+        <v>0.5981925273873964</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.5486607591052849</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
       <c r="F2" t="n">
-        <v>2.0073553136445352</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2.0073553136445352</v>
+        <v>2.2377693211459815</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5618782570667403</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.2088419802184494</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
-        <v>0.5506659598635469</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.23307825885659883</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" t="n">
-        <v>2.739150874892997</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2.739150874892997</v>
+        <v>3.0187694628076245</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>1.9287923881784081</v>
+        <v>1.9783054874278605</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8844663705715717</v>
+        <v>0.8995421954413824</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>11.804550273027079</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="n">
-        <v>11.804550273027079</v>
+        <v>14.539280728964417</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0023716500187338065</v>
+        <v>0.010352502365498943</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09844939610494902</v>
+        <v>0.01230734702769087</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>7.502947515427074</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.09844939610494902</v>
+        <v>0.29473446657327257</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" t="n">
         <v>100.0</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D6" t="n">
         <v>100.0</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F6" t="n">
         <v>100.0</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="n">
-        <v>100.0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" t="n">
-        <v>20.080468362729306</v>
+        <v>6.5192256523457095</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>0.42268366304013083</v>
+        <v>0.3473716857771041</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F7" t="n">
-        <v>1.3577171367384337</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.3577171367384337</v>
+        <v>1.3422463444429102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0635743787662762</v>
+        <v>-0.006954051708289555</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5102028463939461</v>
+        <v>0.5637336006513523</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F8" t="n">
-        <v>1.5553954192871906</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.5553954192871906</v>
+        <v>1.7396723597827235</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B9" t="n">
-        <v>0.11814538798869426</v>
+        <v>0.17846577312373474</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5871186718166237</v>
+        <v>0.6326514541234405</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F9" t="n">
-        <v>2.45931520800188</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2.45931520800188</v>
+        <v>2.7358662825092397</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.30323299935244147</v>
+        <v>0.315707175764358</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05432547475162369</v>
+        <v>0.04361497270156321</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F10" t="n">
-        <v>7.502947515427072</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" t="n">
-        <v>7.502947515427072</v>
+        <v>9.112969069579835</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9300343790091574</v>
+        <v>0.9832735722884536</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9523209941081725</v>
+        <v>0.9917113389539829</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F11" t="n">
-        <v>7.784545404301034</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="n">
-        <v>7.784545404301034</v>
+        <v>10.625527530777841</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.9987580091692507</v>
+        <v>-0.9950319151394069</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D12" t="n">
-        <v>0.06785462353660072</v>
+        <v>0.09216914351260054</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F12" t="n">
-        <v>-4.020004868726046</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" t="n">
-        <v>-4.020004868726046</v>
+        <v>-3.9137531981865763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>